<commit_message>
Atualizando versao do python para o heroku
</commit_message>
<xml_diff>
--- a/data/Nota_Fiscal.xlsx
+++ b/data/Nota_Fiscal.xlsx
@@ -668,10 +668,10 @@
         </is>
       </c>
       <c r="F2" s="9" t="n">
-        <v>45485.40715277778</v>
+        <v>45489.40292824074</v>
       </c>
       <c r="G2" s="9" t="n">
-        <v>45485.40715277778</v>
+        <v>45489.40292824074</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>88113.0</v>
+        <v>88206.0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -688,22 +688,22 @@
       </c>
       <c r="K2" s="15" t="inlineStr">
         <is>
-          <t>100094424</t>
+          <t>100094507</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>BR0015442</t>
+          <t>BR0026113</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>SAO LUIZ ADM SHOPPING S/C LTDA</t>
+          <t>MANGUINHOS ADM DE BENS E CONSULTORI</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>6107</t>
+          <t>6949</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -723,14 +723,14 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
       <c r="S2" t="n">
-        <v>7586.69</v>
+        <v>3503.23</v>
       </c>
       <c r="T2" t="n">
-        <v>7586.69</v>
+        <v>0.0</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
@@ -739,12 +739,12 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Venda com pedido</t>
+          <t>Remessa</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>141240207223659</t>
+          <t>141240210540098</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>100079953</t>
+          <t/>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
@@ -779,42 +779,42 @@
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>41240776881093000172550020000881131000944245</t>
+          <t>41240776881093000172550020000882061000945072</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>001</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>686</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>JAMEF ENCOMENDAS URGENTE</t>
+          <t>BRAVO LOG TRANSPORTES LTDA</t>
         </is>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>BR0014137</t>
+          <t>BR0025169</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>BR0015442</t>
+          <t>BR0026113</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>S101</t>
+          <t>S949</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>BR0101</t>
+          <t>BR0105</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
@@ -833,10 +833,10 @@
         </is>
       </c>
       <c r="F3" s="9" t="n">
-        <v>45485.407164351855</v>
+        <v>45489.403229166666</v>
       </c>
       <c r="G3" s="9" t="n">
-        <v>45485.407164351855</v>
+        <v>45489.403229166666</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -844,7 +844,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>88114.0</v>
+        <v>88207.0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -853,17 +853,17 @@
       </c>
       <c r="K3" s="15" t="inlineStr">
         <is>
-          <t>100094426</t>
+          <t>100094534</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>BR1901219</t>
+          <t>BR1002176</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>IRMAOS KUNST CONSTRUCOES LTDA</t>
+          <t>LOCALIZA RENT A CAR S/A</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -892,10 +892,10 @@
         </is>
       </c>
       <c r="S3" t="n">
-        <v>765.0</v>
+        <v>26019.04</v>
       </c>
       <c r="T3" t="n">
-        <v>765.0</v>
+        <v>26019.04</v>
       </c>
       <c r="U3" t="inlineStr">
         <is>
@@ -909,7 +909,7 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>141240207223424</t>
+          <t>141240210541154</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
@@ -919,12 +919,12 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>100079955</t>
+          <t>100080047</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Por Conta do Destinatário (FOB)</t>
+          <t>Por Conta do Remetente (CIF)</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>FOB</t>
+          <t>CIF</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
@@ -944,32 +944,32 @@
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>41240776881093000172550020000881141000944269</t>
+          <t>41240776881093000172550020000882071000945347</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>130</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>143</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>EXPRESSO SÃO MIGUEL LTDA</t>
+          <t>JAMEF ENCOMENDAS URGENTE</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>BR0005627</t>
+          <t>BR0000131</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr">
         <is>
-          <t>BR1901219</t>
+          <t>BR1002176</t>
         </is>
       </c>
       <c r="AJ3" t="inlineStr">
@@ -998,10 +998,10 @@
         </is>
       </c>
       <c r="F4" s="9" t="n">
-        <v>45485.407175925924</v>
+        <v>45489.40325231481</v>
       </c>
       <c r="G4" s="9" t="n">
-        <v>45485.407175925924</v>
+        <v>45489.40325231481</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1009,7 +1009,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>88115.0</v>
+        <v>88208.0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -1018,17 +1018,17 @@
       </c>
       <c r="K4" s="15" t="inlineStr">
         <is>
-          <t>100094427</t>
+          <t>100094535</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>BR0026573</t>
+          <t>BR0010977</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>I2R STUDIO DE BIKE FORTALEZA LTDA</t>
+          <t>AMB EMPREENDIMENTOS IMOBIL. LTDA</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -1057,10 +1057,10 @@
         </is>
       </c>
       <c r="S4" t="n">
-        <v>363.75</v>
+        <v>42500.24</v>
       </c>
       <c r="T4" t="n">
-        <v>363.75</v>
+        <v>42500.24</v>
       </c>
       <c r="U4" t="inlineStr">
         <is>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>141240207223656</t>
+          <t>141240210541153</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>100079956</t>
+          <t>100080048</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
@@ -1109,32 +1109,32 @@
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>41240776881093000172550020000881151000944274</t>
+          <t>41240776881093000172550020000882081000945352</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>000</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>017</t>
+          <t>E73</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>TRANSJOI TRANSPORTES LTDA.</t>
+          <t>TRANSPORTES RODOVIA SUL LTDA</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>BR0025629</t>
+          <t>BR0009430</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>BR0026573</t>
+          <t>BR0010977</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
@@ -1163,10 +1163,10 @@
         </is>
       </c>
       <c r="F5" s="9" t="n">
-        <v>45485.4071875</v>
+        <v>45489.40326388889</v>
       </c>
       <c r="G5" s="9" t="n">
-        <v>45485.4071875</v>
+        <v>45489.40326388889</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>88116.0</v>
+        <v>88209.0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -1183,136 +1183,631 @@
       </c>
       <c r="K5" s="15" t="inlineStr">
         <is>
-          <t>100094428</t>
+          <t>100094536</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>BR0025553</t>
+          <t>BR1530316</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>UNIMED VITORIA COOPERATIVA DE TRABA</t>
+          <t>IRMAND.STA CASA MISER.PORTO ALEGRE</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
+          <t>6107</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Impresso</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Processada</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Autorizada</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>2534.17</v>
+      </c>
+      <c r="T5" t="n">
+        <v>2534.17</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>BRL</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Venda com pedido</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>141240210541150</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>100080049</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Por Conta do Destinatário (FOB)</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>FOB</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>41240776881093000172550020000882091000945368</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>H72</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>RODONAVES TRANSPORTES E ENC. L</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>BR0004486</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>BR1530316</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>S101</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>BR0101</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="n">
+        <v>460.0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F6" s="9" t="n">
+        <v>45489.40326388889</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>45489.40326388889</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>88210.0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K6" s="15" t="inlineStr">
+        <is>
+          <t>100094537</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>BR1550742</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>FUNDACAO FELICE ROSSO</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
           <t>6949</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>Impresso</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>Processada</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>Autorizada</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="S5" t="n">
-        <v>17.88</v>
-      </c>
-      <c r="T5" t="n">
+      <c r="S6" t="n">
+        <v>726.01</v>
+      </c>
+      <c r="T6" t="n">
         <v>0.0</v>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>BRL</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>Remessa</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>141240207223478</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>100079957</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>141240210540903</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>100080050</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
         <is>
           <t>Por Conta do Remetente (CIF)</t>
         </is>
       </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
         <is>
           <t>CIF</t>
         </is>
       </c>
-      <c r="AC5" t="inlineStr">
+      <c r="AC6" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>41240776881093000172550020000881161000944280</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>41240776881093000172550020000882101000945377</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
         <is>
           <t>999</t>
         </is>
       </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>E13</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>PRESTEX ENCOMENDAS EXPRESSAS L</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>BR0024608</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>BR0025553</t>
-        </is>
-      </c>
-      <c r="AJ5" t="inlineStr">
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>JAMEF ENCOMENDAS URGENTE</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>BR0004535</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>BR1550742</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
         <is>
           <t>S949GR</t>
         </is>
       </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>BR0104</t>
-        </is>
-      </c>
-      <c r="AL5" t="inlineStr">
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>BR0101</t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="n">
+        <v>460.0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F7" s="9" t="n">
+        <v>45489.403275462966</v>
+      </c>
+      <c r="G7" s="9" t="n">
+        <v>45489.403275462966</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>88211.0</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K7" s="15" t="inlineStr">
+        <is>
+          <t>100094538</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>BR0025869</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>CONDOMINIO SOBERANE RESIDENCE, CORP</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>6107</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Impresso</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Processada</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Autorizada</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>6104.71</v>
+      </c>
+      <c r="T7" t="n">
+        <v>6104.71</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>BRL</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Venda com pedido</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>141240210541149</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>100080051</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Por Conta do Destinatário (FOB)</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>FOB</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>41240776881093000172550020000882111000945382</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>001</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>017</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>TRANSJOI TRANSPORTES LTDA.</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>BR0024925</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>BR0025869</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>S101</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>BR0101</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="n">
+        <v>460.0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F8" s="9" t="n">
+        <v>45489.40329861111</v>
+      </c>
+      <c r="G8" s="9" t="n">
+        <v>45489.40329861111</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>88212.0</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K8" s="15" t="inlineStr">
+        <is>
+          <t>100094541</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>BR0015419</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>SPE SAUDE PRIMARIA BH S/A</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>6107</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Impresso</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Processada</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Autorizada</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>73287.71</v>
+      </c>
+      <c r="T8" t="n">
+        <v>73287.71</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>BRL</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Venda com pedido</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>141240210541157</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>100080053</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>Por Conta do Destinatário (FOB)</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>FOB</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>41240776881093000172550020000882121000945410</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>017</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>TRANSJOI TRANSPORTES LTDA.</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>BR0014114</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>BR0015419</t>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>S101</t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>BR0101</t>
+        </is>
+      </c>
+      <c r="AL8" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>